<commit_message>
Dodanie calego repo na nowy komputer
</commit_message>
<xml_diff>
--- a/Python_ksiazka_przyklady/excel/stores.xlsx
+++ b/Python_ksiazka_przyklady/excel/stores.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lestk\Documents\Helion\PfE\Kody\xl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repozytorium\Kody_Python\Python_ksiazka_przyklady\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45442B86-E224-414A-BE74-DB936DF56FD9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12DA904B-0296-4C37-A13B-EF9232748BBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{DE96EA78-DEDB-0845-B68B-3B0A992487D5}"/>
+    <workbookView xWindow="-23148" yWindow="2676" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{DE96EA78-DEDB-0845-B68B-3B0A992487D5}"/>
   </bookViews>
   <sheets>
     <sheet name="2019" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
     <definedName name="IQ_YTD">3000</definedName>
     <definedName name="IQ_YTDMONTH" hidden="1">130000</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -60,6 +60,9 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -193,7 +196,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -209,9 +212,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -249,7 +252,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -355,7 +358,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -508,19 +511,19 @@
   <dimension ref="B2:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.59765625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5" customWidth="1"/>
     <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>15</v>
       </c>
@@ -537,7 +540,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -554,7 +557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -571,7 +574,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -585,7 +588,7 @@
         <v>43861</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -602,7 +605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -616,7 +619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>4</v>
       </c>
@@ -643,17 +646,17 @@
   <dimension ref="B2:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.59765625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>15</v>
       </c>
@@ -670,7 +673,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -687,7 +690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -704,7 +707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -721,7 +724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -735,7 +738,7 @@
         <v>43922</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>6</v>
       </c>
@@ -749,7 +752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>4</v>
       </c>
@@ -776,27 +779,27 @@
   <dimension ref="B1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.59765625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="14.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="2:6" s="4" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:6" s="4" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="6">
         <v>2019</v>
       </c>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>15</v>
       </c>
@@ -813,7 +816,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -830,7 +833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>0</v>
       </c>
@@ -847,7 +850,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>1</v>
       </c>
@@ -861,7 +864,7 @@
         <v>43861</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -878,7 +881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>6</v>
       </c>
@@ -892,7 +895,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>4</v>
       </c>
@@ -909,18 +912,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B13" s="6">
         <v>2020</v>
       </c>
@@ -929,7 +932,7 @@
       <c r="E13" s="4"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>15</v>
       </c>
@@ -946,7 +949,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>2</v>
       </c>
@@ -963,7 +966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>0</v>
       </c>
@@ -980,7 +983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>1</v>
       </c>
@@ -997,7 +1000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>3</v>
       </c>
@@ -1011,7 +1014,7 @@
         <v>43922</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>6</v>
       </c>
@@ -1025,7 +1028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>4</v>
       </c>

</xml_diff>